<commit_message>
update deployment - predict page - file upload
</commit_message>
<xml_diff>
--- a/deployment/result.xlsx
+++ b/deployment/result.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,46 +497,442 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>29</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>18</v>
+      </c>
+      <c r="D2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
         <v>30</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Premium</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Quarterly</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>930</v>
+      </c>
+      <c r="J2" t="n">
+        <v>18</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>39</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C3" t="n">
         <v>12</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Quarterly</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>969</v>
+      </c>
+      <c r="J3" t="n">
+        <v>13</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>30</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>39</v>
+      </c>
+      <c r="D4" t="n">
+        <v>14</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" t="n">
+        <v>18</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Annual</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>932</v>
+      </c>
+      <c r="J4" t="n">
+        <v>17</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>23</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>32</v>
+      </c>
+      <c r="D5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Monthly</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>617</v>
+      </c>
+      <c r="J5" t="n">
+        <v>20</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>65</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>49</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
         <v>10</v>
       </c>
-      <c r="E2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="F6" t="n">
+        <v>8</v>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>Basic</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Monthly</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>100</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="I6" t="n">
+        <v>557</v>
+      </c>
+      <c r="J6" t="n">
+        <v>6</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>55</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>14</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" t="n">
+        <v>6</v>
+      </c>
+      <c r="F7" t="n">
+        <v>18</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Quarterly</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>185</v>
+      </c>
+      <c r="J7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>58</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>38</v>
+      </c>
+      <c r="D8" t="n">
+        <v>21</v>
+      </c>
+      <c r="E8" t="n">
         <v>7</v>
       </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
+      <c r="F8" t="n">
+        <v>7</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Monthly</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>396</v>
+      </c>
+      <c r="J8" t="n">
+        <v>29</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>58</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>49</v>
+      </c>
+      <c r="D9" t="n">
+        <v>12</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" t="n">
+        <v>16</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Quarterly</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>821</v>
+      </c>
+      <c r="J9" t="n">
+        <v>24</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>55</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>37</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" t="n">
+        <v>15</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Premium</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Annual</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>445</v>
+      </c>
+      <c r="J10" t="n">
+        <v>30</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>64</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>25</v>
+      </c>
+      <c r="E11" t="n">
         <v>2</v>
+      </c>
+      <c r="F11" t="n">
+        <v>11</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Quarterly</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>415</v>
+      </c>
+      <c r="J11" t="n">
+        <v>29</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>